<commit_message>
Build site at 2021-10-27 12:19:33 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOB1057.xlsx
+++ b/assets/disciplinas/LOB1057.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Ementa atual:</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Semestre ideal:</t>
   </si>
   <si>
-    <t>EP-8</t>
+    <t>EA-8,EP-8</t>
   </si>
   <si>
     <t>Objetivos:</t>
@@ -128,13 +128,6 @@
   </si>
   <si>
     <t>ABRAÃO, J et al. Introdução à Ergonomia: da Prática à Teoria. São Paulo: Edgard Blücher, 2009.COUTO, H.A. Como implantar a ergonomia na empresa. Belo Horizonte: Ergo Editora, 2002.DUL, J.; WEERDMEESTER, B. Ergonomia prática. São Paulo: Edgard Blücher, 2004.GRANDJEAN, E. Manual de Ergonomia. 5ª ed. Porto Alegre; Bookman, 2004.GUÉRIN, E et al. Compreender o trabalho para transformá-lo. São Paulo: Edgard Blücher, 2001. IIDA, I. Ergonomia: Projeto e Produção - 2º edição revista e ampliada. São Paulo: Edgard Blucher, 2005.MÁSCULO, F.S.; VIDAL, N.C.(Org.). Ergonomia: trabalho adequado e eficiente. Rio de Janeiro: Elsevier, 2011.SANTOS, N.; FIALHO, F.A.P., Manual de Análise Ergonômica no Trabalho. Curitiba: Gênesis Editora, 2a. Ed., 1997.VIDAL, M.C. Ergonomia na empresa, útil, prática e aplicada, 2º ed. Rio de Janeiro: Editora CVC, 2002. VIDAL, M.C.; CARVALHO, P.V.R. Ergonomia cognitiva: raciocínio e decisão no trabalho. Rio de Janeiro: Ed. Virtual Científica, 2008.Artigos selecionados pelos Docentes</t>
-  </si>
-  <si>
-    <t>Requisitos:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOQ4205 -  Sistemas Produtivos II  (Requisito fraco)
-</t>
   </si>
 </sst>
 </file>
@@ -490,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -712,19 +705,6 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1">
-      <c r="B25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>